<commit_message>
* final adaptions * timelog
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="5055" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="5505" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>preparing presentation</t>
+  </si>
+  <si>
+    <t>preparing for presentation</t>
+  </si>
+  <si>
+    <t>conducting presentation</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +807,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>42291</v>
+        <v>41927</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -818,21 +824,39 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="2">
+        <v>41927</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D22" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="2">
+        <v>41927</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
* copied and adapted expose * renamed some sections
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="13155" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="13575" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>tri dexel implementation</t>
+  </si>
+  <si>
+    <t>thesis chapter introduction</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1680,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ref="D67:D88" si="2">C67-B67</f>
+        <f t="shared" ref="D67:D92" si="2">C67-B67</f>
         <v>5.2083333333333259E-2</v>
       </c>
       <c r="E67" t="s">
@@ -2063,28 +2066,76 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="3"/>
+      <c r="A89" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B89" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C89" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="2"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E89" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="3"/>
+      <c r="A90" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B90" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C90" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="2"/>
+        <v>0.12499999999999994</v>
+      </c>
+      <c r="E90" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="3"/>
+      <c r="A91" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C91" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="2"/>
+        <v>0.12500000000000006</v>
+      </c>
+      <c r="E91" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="3"/>
+      <c r="A92" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B92" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="C92" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="2"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E92" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
@@ -2095,7 +2146,7 @@
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D94" s="4">
         <f>SUM(D2:D93)</f>
-        <v>9.6562500000000018</v>
+        <v>10.13541666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished dexel, multi-dexel and CSG description
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="14025" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="14475" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
   <si>
     <t>date</t>
   </si>
@@ -473,7 +473,7 @@
   <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1683,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ref="D67:D94" si="2">C67-B67</f>
+        <f t="shared" ref="D67:D96" si="2">C67-B67</f>
         <v>5.2083333333333259E-2</v>
       </c>
       <c r="E67" t="s">
@@ -2176,10 +2176,93 @@
         <v>31</v>
       </c>
     </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>42115</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C95" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="E95" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>42115</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C96" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="2"/>
+        <v>0.21875</v>
+      </c>
+      <c r="E96" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>42116</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C97" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E97" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+    </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="4">
         <f>SUM(D2:D123)</f>
-        <v>10.38541666666667</v>
+        <v>10.63541666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished terms in fundamentals
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="14925" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="15375" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="34">
   <si>
     <t>date</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>thesis chapter fundamentals, surface representations and terms</t>
+  </si>
+  <si>
+    <t>thesis chapter fundamentals, terms</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,17 +2255,39 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
+      <c r="A99" s="2">
+        <v>42120</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C99" s="5">
+        <v>0.625</v>
+      </c>
       <c r="D99" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="E99" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
+      <c r="A100" s="2">
+        <v>42120</v>
+      </c>
+      <c r="B100" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C100" s="5">
+        <v>0.8125</v>
+      </c>
       <c r="D100" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E100" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,7 +2439,7 @@
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="4">
         <f>SUM(D2:D123)</f>
-        <v>11.069444444444446</v>
+        <v>11.381944444444446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continued and finished chapter previous work
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="16725" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="17175" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
   <si>
     <t>date</t>
   </si>
@@ -491,7 +491,7 @@
   <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,29 +2411,75 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
+      <c r="A107" s="2">
+        <v>42123</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C107" s="5">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="D107" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="E107" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
+      <c r="A108" s="2">
+        <v>42123</v>
+      </c>
+      <c r="B108" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C108" s="5">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="D108" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="E108" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>42124</v>
+      </c>
+      <c r="B109" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C109" s="5">
+        <v>0.53125</v>
+      </c>
       <c r="D109" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>42124</v>
+      </c>
+      <c r="B110" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="C110" s="5">
+        <v>0.75</v>
+      </c>
       <c r="D110" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.17708333333333337</v>
+      </c>
+      <c r="E110" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,7 +2563,7 @@
     <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="4">
         <f>SUM(D2:D123)</f>
-        <v>11.875000000000002</v>
+        <v>12.500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* fixed classification figure * timelog
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="17175" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="17625" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>thesis chapter previous work</t>
+  </si>
+  <si>
+    <t>thesis chapter state of the art</t>
   </si>
 </sst>
 </file>
@@ -490,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,87 +2486,147 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>42125</v>
+      </c>
+      <c r="B111" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C111" s="5">
+        <v>1</v>
+      </c>
       <c r="D111" s="3">
         <f t="shared" si="2"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E111" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>42126</v>
+      </c>
+      <c r="B112" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C112" s="5">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="D112" s="3">
         <f t="shared" si="2"/>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E112" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+      <c r="D121" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
       <c r="D124" s="4">
         <f>SUM(D2:D123)</f>
-        <v>12.500000000000002</v>
+        <v>12.645833333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* some notes in direct_intersection.tex * timelog
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20295" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="20745" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>raycasting image by thorsten</t>
+  </si>
+  <si>
+    <t>integrated Geometric Tools Library for direct intersection</t>
+  </si>
+  <si>
+    <t>stabilizing direct intersection</t>
+  </si>
+  <si>
+    <t>rewriting direct intersection to operate per cell</t>
   </si>
 </sst>
 </file>
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1768,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ref="D67:D150" si="2">C67-B67</f>
+        <f t="shared" ref="D67:D154" si="2">C67-B67</f>
         <v>5.2083333333333259E-2</v>
       </c>
       <c r="E67" t="s">
@@ -3258,6 +3267,78 @@
       </c>
       <c r="E150" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>42181</v>
+      </c>
+      <c r="B151" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C151" s="5">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D151" s="3">
+        <f t="shared" si="2"/>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="E151" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>42184</v>
+      </c>
+      <c r="B152" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C152" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D152" s="3">
+        <f t="shared" si="2"/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="E152" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>42185</v>
+      </c>
+      <c r="B153" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C153" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D153" s="3">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="E153" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>42185</v>
+      </c>
+      <c r="B154" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="C154" s="5">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D154" s="3">
+        <f t="shared" si="2"/>
+        <v>0.23958333333333337</v>
+      </c>
+      <c r="E154" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3285,7 +3366,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(individuals!D2:D1000)</f>
-        <v>17.138888888888889</v>
+        <v>18.003472222222221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* changed chapter titles of bpa and tri dexel * added line spacing for wbackfrieder * timelog
</commit_message>
<xml_diff>
--- a/documents/timelog.xlsx
+++ b/documents/timelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="27495" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="28095" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="individuals" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="85">
   <si>
     <t>date</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>proofreading direct intersection</t>
+  </si>
+  <si>
+    <t>proofreading whole thesis using MS Word, releasing to wbackfrieder</t>
   </si>
 </sst>
 </file>
@@ -629,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="E216" sqref="E216"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4422,9 +4425,21 @@
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>42254</v>
+      </c>
+      <c r="B211" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C211" s="5">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D211" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.1875</v>
+      </c>
+      <c r="E211" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4728,7 +4743,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(individuals!D2:D1000)</f>
-        <v>24.329861111111104</v>
+        <v>24.517361111111104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>